<commit_message>
Start bringing in blazor samples
</commit_message>
<xml_diff>
--- a/Planning & Analysis.xlsx
+++ b/Planning & Analysis.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\shinyorg\shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E17F89A-D9B3-4599-A4FA-1F7C9AD6E434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EFD8D7-D170-4E25-9BE3-700FC59578D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FBA5338F-6A38-496E-92DE-5CE895C325C0}"/>
+    <workbookView xWindow="2540" yWindow="3320" windowWidth="28800" windowHeight="15370" activeTab="4" xr2:uid="{FBA5338F-6A38-496E-92DE-5CE895C325C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Feature Analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Platform" sheetId="2" r:id="rId2"/>
-    <sheet name="Feature Movement" sheetId="5" r:id="rId3"/>
-    <sheet name="Blocked Features" sheetId="6" r:id="rId4"/>
-    <sheet name="Framework" sheetId="8" r:id="rId5"/>
+    <sheet name="Blazor" sheetId="9" r:id="rId2"/>
+    <sheet name="Platform" sheetId="2" r:id="rId3"/>
+    <sheet name="Feature Movement" sheetId="5" r:id="rId4"/>
+    <sheet name="Blocked Features" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="108">
   <si>
     <t>Startup</t>
   </si>
@@ -116,12 +116,6 @@
     <t>If using direct GPS</t>
   </si>
   <si>
-    <t>mDNS Broadcasting</t>
-  </si>
-  <si>
-    <t>iOS Push Notification Interceptor (Location &amp; Mutator)</t>
-  </si>
-  <si>
     <t>Shiny Task</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>Persisted State</t>
   </si>
   <si>
-    <t>Persisted State requires control over DI startup</t>
-  </si>
-  <si>
     <t>MAYBE in future</t>
   </si>
   <si>
@@ -203,9 +194,6 @@
     <t>Configuration Extensions</t>
   </si>
   <si>
-    <t>User Dialogs</t>
-  </si>
-  <si>
     <t>Shiny.Push.FirebaseMessaging</t>
   </si>
   <si>
@@ -254,9 +242,6 @@
     <t>Shiny.Logging.AppCenter</t>
   </si>
   <si>
-    <t>iOS 3rd Party</t>
-  </si>
-  <si>
     <t>AppCenter</t>
   </si>
   <si>
@@ -290,9 +275,6 @@
     <t>Function</t>
   </si>
   <si>
-    <t>Localization</t>
-  </si>
-  <si>
     <t>Connectivity</t>
   </si>
   <si>
@@ -311,24 +293,6 @@
     <t>Needed only by foreground event</t>
   </si>
   <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>ViewModel</t>
-  </si>
-  <si>
-    <t>Prism Integration</t>
-  </si>
-  <si>
-    <t>ReactiveUI Integration</t>
-  </si>
-  <si>
-    <t>Validation</t>
-  </si>
-  <si>
-    <t>Message Bus is bonus feature</t>
-  </si>
-  <si>
     <t>Configuration</t>
   </si>
   <si>
@@ -347,21 +311,12 @@
     <t>Maybe for iOS dialogs</t>
   </si>
   <si>
-    <t>Above chart is to help determine necessity of hosting for each plugin or to split hosting out?</t>
-  </si>
-  <si>
     <t>Background Listening??</t>
   </si>
   <si>
     <t>Deprecated</t>
   </si>
   <si>
-    <t>Startups are usually to write delegates before system spins up</t>
-  </si>
-  <si>
-    <t>Anything requiring repository or permissions - needs platform</t>
-  </si>
-  <si>
     <t>Browser (ie. Edge - Microsoft?)</t>
   </si>
   <si>
@@ -387,6 +342,24 @@
   </si>
   <si>
     <t>????</t>
+  </si>
+  <si>
+    <t>Push</t>
+  </si>
+  <si>
+    <t>Notifications</t>
+  </si>
+  <si>
+    <t>BluetoothLE</t>
+  </si>
+  <si>
+    <t>Locations - GPS only</t>
+  </si>
+  <si>
+    <t>Core - Connectivity</t>
+  </si>
+  <si>
+    <t>Core - Battery</t>
   </si>
 </sst>
 </file>
@@ -584,21 +557,11 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D345163C-329F-4566-A5B5-E3E179D5F2FD}" name="Table6" displayName="Table6" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5" xr:uid="{D345163C-329F-4566-A5B5-E3E179D5F2FD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D345163C-329F-4566-A5B5-E3E179D5F2FD}" name="Table6" displayName="Table6" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4" xr:uid="{D345163C-329F-4566-A5B5-E3E179D5F2FD}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{32A59D28-B3DE-49D6-BD3F-563E01BE0CAC}" name="Library"/>
     <tableColumn id="2" xr3:uid="{66CBF6D9-CCC4-4C1A-84BD-7E9B50D7C93E}" name="Reason"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0A581705-4D72-824D-A6CE-A77ABD5CCABF}" name="Table2" displayName="Table2" ref="A1:A6" totalsRowShown="0">
-  <autoFilter ref="A1:A6" xr:uid="{0A581705-4D72-824D-A6CE-A77ABD5CCABF}"/>
-  <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{83426C67-69DE-4E44-8DC1-717D15558371}" name="Feature"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -901,31 +864,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6DD48B-CA33-4E1C-94C3-D30E7253B570}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="33.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.453125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" customWidth="1"/>
+    <col min="6" max="6" width="24.7265625" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
+    <col min="8" max="8" width="18.7265625" customWidth="1"/>
+    <col min="9" max="9" width="18.26953125" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" customWidth="1"/>
+    <col min="12" max="12" width="12.453125" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" customWidth="1"/>
+    <col min="14" max="14" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -942,34 +905,34 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
         <v>21</v>
       </c>
       <c r="I1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" t="s">
         <v>85</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>86</v>
       </c>
-      <c r="L1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M1" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -983,7 +946,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>18</v>
@@ -995,13 +958,13 @@
         <v>18</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1020,14 +983,14 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="4" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1042,10 +1005,10 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
@@ -1059,13 +1022,13 @@
         <v>18</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1081,7 +1044,7 @@
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
@@ -1094,16 +1057,16 @@
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>101</v>
-      </c>
       <c r="N5" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1111,7 +1074,7 @@
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="2" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -1128,14 +1091,14 @@
         <v>18</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1159,13 +1122,13 @@
         <v>18</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1192,10 +1155,10 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1220,16 +1183,16 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="N9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1254,14 +1217,14 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1293,7 +1256,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1321,7 +1284,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1330,7 +1293,7 @@
         <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1347,9 +1310,9 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>18</v>
@@ -1358,7 +1321,7 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>18</v>
@@ -1370,12 +1333,12 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="1" t="s">
@@ -1397,81 +1360,46 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1483,6 +1411,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EFCFB6-B898-4223-A372-DBB251926B4A}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD3C381B-CFB3-4346-B649-B6650CD75C64}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -1490,38 +1483,38 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="1"/>
@@ -1529,9 +1522,9 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="1"/>
@@ -1539,9 +1532,9 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="1"/>
@@ -1549,107 +1542,107 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>48</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="1"/>
@@ -1657,138 +1650,29 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D45D83-9BCF-41F3-AEEE-6B23534485CE}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="91.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" t="s">
-        <v>80</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1799,56 +1683,103 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6466D272-45F0-4444-A1DD-F69955F3D21A}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D45D83-9BCF-41F3-AEEE-6B23534485CE}">
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.26953125" customWidth="1"/>
+    <col min="2" max="2" width="91.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B8" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C8" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1861,46 +1792,49 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AC4FEE0-6D69-435A-83EC-A0F4FA0436C3}">
-  <dimension ref="A1:A6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6466D272-45F0-4444-A1DD-F69955F3D21A}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>93</v>
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>